<commit_message>
+zrób excel z wynikami
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel.xlsx
+++ b/src/main/resources/Excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Imię</t>
   </si>
@@ -38,7 +38,7 @@
     <t>99087666341</t>
   </si>
   <si>
-    <t>Idź na badanie</t>
+    <t>Nie stać Cię na test - GIŃ</t>
   </si>
   <si>
     <t>Mikołaj</t>
@@ -50,6 +50,9 @@
     <t>12345678910</t>
   </si>
   <si>
+    <t>Wynik testu na obecność korona wirusa pozytywny</t>
+  </si>
+  <si>
     <t>Jan</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t>82345678910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wynik testu na obecność korona wirusa negatywny </t>
   </si>
   <si>
     <t>Test</t>
@@ -155,38 +161,38 @@
         <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>320.0</v>
+        <v>190.0</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>700.0</v>
+        <v>570.0</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
       <c r="D5" t="n">
         <v>123.0</v>

</xml_diff>